<commit_message>
* Added Example use case \ * Modified use case template
</commit_message>
<xml_diff>
--- a/docs/usecases/Use Case Template.xlsx
+++ b/docs/usecases/Use Case Template.xlsx
@@ -15,17 +15,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
-  <si>
-    <t>User Case:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+  <si>
+    <t>Use Case:</t>
   </si>
   <si>
     <t>Short description:</t>
   </si>
   <si>
+    <t>Goal</t>
+  </si>
+  <si>
     <t>Person involved:</t>
   </si>
   <si>
+    <t>Trigger</t>
+  </si>
+  <si>
     <t>Precondition:</t>
   </si>
   <si>
@@ -54,9 +60,6 @@
   </si>
   <si>
     <t>Alternative use case:</t>
-  </si>
-  <si>
-    <t>Quality Requirements:</t>
   </si>
   <si>
     <t>User Case Template V1.5</t>
@@ -69,7 +72,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -102,14 +105,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="15"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF44546A"/>
       <name val="Calibri"/>
@@ -141,12 +136,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF1F4E79"/>
         <bgColor rgb="FF44546A"/>
       </patternFill>
@@ -169,8 +158,14 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -183,12 +178,26 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color rgb="FF5B9BD5"/>
+        <color rgb="FFADCDEA"/>
       </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="medium"/>
+      <right/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -198,6 +207,29 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF9DC3E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
       <right/>
       <top/>
       <bottom style="thick">
@@ -206,54 +238,8 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium"/>
-      <top style="medium"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF9DC3E6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF9DC3E6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
       <top/>
       <bottom style="thick">
         <color rgb="FFADCDEA"/>
@@ -261,30 +247,21 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="medium"/>
       <top/>
-      <bottom style="thick">
-        <color rgb="FFADCDEA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right/>
-      <top/>
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="medium"/>
-      <top/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,92 +285,80 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="11" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 3" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -413,7 +378,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFADCDEA"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF5B9BD5"/>
+      <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFDEEBF7"/>
@@ -463,173 +428,156 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C27"/>
+  <dimension ref="B2:C65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.556122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.3367346938775"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="61.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.89285714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="0.556122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3367346938775"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.89285714285714"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-    </row>
     <row r="2" customFormat="false" ht="19.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6" t="s">
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="10" t="s">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="11"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="9"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12" t="s">
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="s">
+      <c r="B20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="11"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="9"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
+      <c r="C24" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>